<commit_message>
table of contents update
</commit_message>
<xml_diff>
--- a/Table of Contents.xlsx
+++ b/Table of Contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/mgardens_calpoly_edu/Documents/Documents/5 Hobbies/1 Coding/Mechatronics Codebases/ME 507 Codebase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_88ECEB8F233FFE205E1D4EF66F09B3AC2A5FD379" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3F534C5-56EF-40D9-ADC3-8E145A84C7DD}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_88ECEB8F233FFE205E1D4EF66F09B3AC2A5FD379" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B90BF0D-AAFF-49F6-99CB-E7D30D763784}"/>
   <bookViews>
     <workbookView xWindow="15934" yWindow="2331" windowWidth="12189" windowHeight="13826" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$8</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -129,7 +140,7 @@
     <t>test-19</t>
   </si>
   <si>
-    <t>RC, closed loop control</t>
+    <t>RC, closed loop control &amp;&amp; Servo</t>
   </si>
 </sst>
 </file>
@@ -508,7 +519,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>